<commit_message>
Loop differential expression between clusters analysis
</commit_message>
<xml_diff>
--- a/CITEseqHIVE_scRNAseq_Pipeline/ScTypeDB_full_MLedit.xlsx
+++ b/CITEseqHIVE_scRNAseq_Pipeline/ScTypeDB_full_MLedit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/monikalooney/Library/CloudStorage/Dropbox/SATVI/SATVI_GitHub/M72_CITEseqHIVE_scRNAseq_Pipeline/CITEseqHIVE_scRNAseq_Pipeline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{41A99A05-D9B0-1F4F-AEF2-C2F124364BD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3632FFF-EA99-6542-9AEA-BDBA7C874CBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="500" windowWidth="23240" windowHeight="14000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="530">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="536">
   <si>
     <t>tissueType</t>
   </si>
@@ -1618,6 +1618,24 @@
   </si>
   <si>
     <t>RP11-104L21.3,BEST3,HKDC1,KLRC4-KLRK1,RP11-305P22.9,LTA,TMSB15B,RP11-739G5.1,UBASH3A,PLK4,FBXO41,LIN28B,SKA3,CD40LG,AC002454.1</t>
+  </si>
+  <si>
+    <t>CD3,CD4,CD69,CD154</t>
+  </si>
+  <si>
+    <t>CD3,CD8,CD69,CD137</t>
+  </si>
+  <si>
+    <t>Activated CD4+ T cells</t>
+  </si>
+  <si>
+    <t>Activated CD8+ T cells</t>
+  </si>
+  <si>
+    <t>Activated CD4+</t>
+  </si>
+  <si>
+    <t>Activated CD8+</t>
   </si>
 </sst>
 </file>
@@ -2012,10 +2030,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E242"/>
+  <dimension ref="A1:E244"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="76" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" zoomScale="76" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57:XFD57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2564,33 +2582,33 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>73</v>
+      <c r="A35" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>532</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>530</v>
       </c>
       <c r="D35" s="4"/>
-      <c r="E35" s="4" t="s">
-        <v>315</v>
+      <c r="E35" s="2" t="s">
+        <v>534</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>75</v>
+      <c r="A36" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>531</v>
       </c>
       <c r="D36" s="4"/>
-      <c r="E36" s="4" t="s">
-        <v>316</v>
+      <c r="E36" s="2" t="s">
+        <v>535</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -2598,14 +2616,14 @@
         <v>71</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D37" s="4"/>
       <c r="E37" s="4" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -2613,14 +2631,14 @@
         <v>71</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D38" s="4"/>
       <c r="E38" s="4" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -2628,14 +2646,14 @@
         <v>71</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D39" s="4"/>
       <c r="E39" s="4" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -2643,14 +2661,14 @@
         <v>71</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>6</v>
+        <v>78</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D40" s="4"/>
       <c r="E40" s="4" t="s">
-        <v>307</v>
+        <v>318</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -2658,14 +2676,14 @@
         <v>71</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -2673,14 +2691,14 @@
         <v>71</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>85</v>
+        <v>6</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="4" t="s">
-        <v>321</v>
+        <v>307</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
@@ -2688,14 +2706,14 @@
         <v>71</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>21</v>
+        <v>83</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>226</v>
+        <v>84</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="4" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
@@ -2703,14 +2721,14 @@
         <v>71</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>67</v>
+        <v>86</v>
       </c>
       <c r="D44" s="4"/>
       <c r="E44" s="4" t="s">
-        <v>303</v>
+        <v>321</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
@@ -2718,14 +2736,14 @@
         <v>71</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>87</v>
+        <v>21</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>88</v>
+        <v>226</v>
       </c>
       <c r="D45" s="4"/>
       <c r="E45" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
@@ -2733,14 +2751,14 @@
         <v>71</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>89</v>
+        <v>66</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="D46" s="4"/>
       <c r="E46" s="4" t="s">
-        <v>324</v>
+        <v>303</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
@@ -2748,14 +2766,14 @@
         <v>71</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D47" s="4"/>
       <c r="E47" s="4" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
@@ -2763,44 +2781,44 @@
         <v>71</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D48" s="4"/>
       <c r="E48" s="4" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>51</v>
+        <v>91</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>52</v>
+        <v>92</v>
       </c>
       <c r="D49" s="4"/>
       <c r="E49" s="4" t="s">
-        <v>51</v>
+        <v>325</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>3</v>
+        <v>93</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>53</v>
+        <v>94</v>
       </c>
       <c r="D50" s="4"/>
       <c r="E50" s="4" t="s">
-        <v>189</v>
+        <v>326</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
@@ -2808,14 +2826,14 @@
         <v>50</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D51" s="4"/>
       <c r="E51" s="4" t="s">
-        <v>327</v>
+        <v>51</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
@@ -2823,14 +2841,14 @@
         <v>50</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>56</v>
+        <v>3</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D52" s="4"/>
       <c r="E52" s="4" t="s">
-        <v>328</v>
+        <v>189</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
@@ -2838,14 +2856,14 @@
         <v>50</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D53" s="4"/>
       <c r="E53" s="4" t="s">
-        <v>58</v>
+        <v>327</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
@@ -2853,14 +2871,14 @@
         <v>50</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D54" s="4"/>
       <c r="E54" s="4" t="s">
-        <v>60</v>
+        <v>328</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
@@ -2868,14 +2886,14 @@
         <v>50</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>233</v>
+        <v>59</v>
       </c>
       <c r="D55" s="4"/>
       <c r="E55" s="4" t="s">
-        <v>322</v>
+        <v>58</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
@@ -2883,14 +2901,14 @@
         <v>50</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D56" s="4"/>
       <c r="E56" s="4" t="s">
-        <v>329</v>
+        <v>60</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
@@ -2898,14 +2916,14 @@
         <v>50</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>64</v>
+        <v>21</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>65</v>
+        <v>233</v>
       </c>
       <c r="D57" s="4"/>
       <c r="E57" s="4" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
@@ -2913,14 +2931,14 @@
         <v>50</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D58" s="4"/>
       <c r="E58" s="4" t="s">
-        <v>303</v>
+        <v>329</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
@@ -2928,14 +2946,14 @@
         <v>50</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>4</v>
+        <v>64</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D59" s="4"/>
       <c r="E59" s="4" t="s">
-        <v>4</v>
+        <v>330</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
@@ -2943,44 +2961,44 @@
         <v>50</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>290</v>
+        <v>67</v>
       </c>
       <c r="D60" s="4"/>
       <c r="E60" s="4" t="s">
-        <v>69</v>
+        <v>303</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
-        <v>109</v>
+        <v>50</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>110</v>
+        <v>4</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>111</v>
+        <v>68</v>
       </c>
       <c r="D61" s="4"/>
       <c r="E61" s="4" t="s">
-        <v>331</v>
+        <v>4</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
-        <v>109</v>
+        <v>50</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>8</v>
+        <v>69</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>112</v>
+        <v>290</v>
       </c>
       <c r="D62" s="4"/>
       <c r="E62" s="4" t="s">
-        <v>8</v>
+        <v>69</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
@@ -2988,14 +3006,14 @@
         <v>109</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D63" s="4"/>
       <c r="E63" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
@@ -3003,14 +3021,14 @@
         <v>109</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>115</v>
+        <v>8</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D64" s="4"/>
       <c r="E64" s="4" t="s">
-        <v>333</v>
+        <v>8</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
@@ -3018,14 +3036,14 @@
         <v>109</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D65" s="4"/>
       <c r="E65" s="4" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
@@ -3033,14 +3051,14 @@
         <v>109</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D66" s="4"/>
       <c r="E66" s="4" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
@@ -3048,14 +3066,14 @@
         <v>109</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D67" s="4"/>
       <c r="E67" s="4" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
@@ -3063,14 +3081,14 @@
         <v>109</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>234</v>
+        <v>120</v>
       </c>
       <c r="D68" s="4"/>
       <c r="E68" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
@@ -3078,14 +3096,14 @@
         <v>109</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>235</v>
+        <v>122</v>
       </c>
       <c r="D69" s="4"/>
       <c r="E69" s="4" t="s">
-        <v>337</v>
+        <v>343</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
@@ -3093,14 +3111,14 @@
         <v>109</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>24</v>
+        <v>123</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>125</v>
+        <v>234</v>
       </c>
       <c r="D70" s="4"/>
       <c r="E70" s="4" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
@@ -3108,14 +3126,14 @@
         <v>109</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>127</v>
+        <v>235</v>
       </c>
       <c r="D71" s="4"/>
       <c r="E71" s="4" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
@@ -3123,14 +3141,14 @@
         <v>109</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>128</v>
+        <v>24</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D72" s="4"/>
       <c r="E72" s="4" t="s">
-        <v>128</v>
+        <v>338</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
@@ -3138,14 +3156,14 @@
         <v>109</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D73" s="4"/>
       <c r="E73" s="4" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
@@ -3153,14 +3171,14 @@
         <v>109</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D74" s="4"/>
       <c r="E74" s="4" t="s">
-        <v>341</v>
+        <v>128</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
@@ -3168,14 +3186,14 @@
         <v>109</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>285</v>
+        <v>131</v>
       </c>
       <c r="D75" s="4"/>
       <c r="E75" s="4" t="s">
-        <v>322</v>
+        <v>340</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
@@ -3183,14 +3201,14 @@
         <v>109</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>70</v>
+        <v>132</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D76" s="4"/>
       <c r="E76" s="4" t="s">
-        <v>70</v>
+        <v>341</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
@@ -3198,14 +3216,14 @@
         <v>109</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>6</v>
+        <v>134</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>136</v>
+        <v>285</v>
       </c>
       <c r="D77" s="4"/>
       <c r="E77" s="4" t="s">
-        <v>189</v>
+        <v>322</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
@@ -3213,14 +3231,14 @@
         <v>109</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>5</v>
+        <v>70</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D78" s="4"/>
       <c r="E78" s="4" t="s">
-        <v>5</v>
+        <v>70</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
@@ -3228,14 +3246,14 @@
         <v>109</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>138</v>
+        <v>6</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D79" s="4"/>
       <c r="E79" s="4" t="s">
-        <v>342</v>
+        <v>189</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
@@ -3243,14 +3261,14 @@
         <v>109</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>140</v>
+        <v>5</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D80" s="4"/>
       <c r="E80" s="4" t="s">
-        <v>344</v>
+        <v>5</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
@@ -3258,14 +3276,14 @@
         <v>109</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D81" s="4"/>
       <c r="E81" s="4" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
@@ -3273,14 +3291,14 @@
         <v>109</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D82" s="4"/>
       <c r="E82" s="4" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
@@ -3288,44 +3306,44 @@
         <v>109</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D83" s="4"/>
       <c r="E83" s="4" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
-        <v>150</v>
+        <v>109</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D84" s="4"/>
       <c r="E84" s="4" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
-        <v>150</v>
+        <v>109</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>283</v>
+        <v>147</v>
       </c>
       <c r="D85" s="4"/>
       <c r="E85" s="4" t="s">
-        <v>322</v>
+        <v>347</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
@@ -3333,14 +3351,14 @@
         <v>150</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D86" s="4"/>
       <c r="E86" s="4" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
@@ -3348,14 +3366,14 @@
         <v>150</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>154</v>
+        <v>283</v>
       </c>
       <c r="D87" s="4"/>
       <c r="E87" s="4" t="s">
-        <v>350</v>
+        <v>322</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
@@ -3363,14 +3381,14 @@
         <v>150</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D88" s="4"/>
       <c r="E88" s="4" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
@@ -3378,14 +3396,14 @@
         <v>150</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D89" s="4"/>
       <c r="E89" s="4" t="s">
-        <v>157</v>
+        <v>350</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
@@ -3393,14 +3411,14 @@
         <v>150</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D90" s="4"/>
       <c r="E90" s="4" t="s">
-        <v>159</v>
+        <v>351</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
@@ -3408,14 +3426,14 @@
         <v>150</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D91" s="4"/>
       <c r="E91" s="4" t="s">
-        <v>353</v>
+        <v>157</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
@@ -3423,14 +3441,14 @@
         <v>150</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D92" s="4"/>
       <c r="E92" s="4" t="s">
-        <v>304</v>
+        <v>159</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
@@ -3438,14 +3456,14 @@
         <v>150</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D93" s="4"/>
       <c r="E93" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
@@ -3453,14 +3471,14 @@
         <v>150</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D94" s="4"/>
       <c r="E94" s="4" t="s">
-        <v>355</v>
+        <v>304</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
@@ -3468,14 +3486,14 @@
         <v>150</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>6</v>
+        <v>165</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D95" s="4"/>
       <c r="E95" s="4" t="s">
-        <v>189</v>
+        <v>354</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
@@ -3483,14 +3501,14 @@
         <v>150</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D96" s="4"/>
       <c r="E96" s="4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
@@ -3498,14 +3516,14 @@
         <v>150</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>172</v>
+        <v>6</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D97" s="4"/>
       <c r="E97" s="4" t="s">
-        <v>357</v>
+        <v>189</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
@@ -3513,14 +3531,14 @@
         <v>150</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D98" s="4"/>
       <c r="E98" s="4" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
@@ -3528,14 +3546,14 @@
         <v>150</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D99" s="4"/>
       <c r="E99" s="4" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
@@ -3543,14 +3561,14 @@
         <v>150</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D100" s="4"/>
       <c r="E100" s="4" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
@@ -3558,14 +3576,14 @@
         <v>150</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D101" s="4"/>
       <c r="E101" s="4" t="s">
-        <v>327</v>
+        <v>359</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
@@ -3573,14 +3591,14 @@
         <v>150</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D102" s="4"/>
       <c r="E102" s="4" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
@@ -3588,14 +3606,14 @@
         <v>150</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D103" s="4"/>
       <c r="E103" s="4" t="s">
-        <v>362</v>
+        <v>327</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
@@ -3603,44 +3621,44 @@
         <v>150</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>148</v>
+        <v>182</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>149</v>
+        <v>183</v>
       </c>
       <c r="D104" s="4"/>
       <c r="E104" s="4" t="s">
-        <v>348</v>
+        <v>361</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" s="4" t="s">
-        <v>7</v>
+        <v>150</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>8</v>
+        <v>184</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>9</v>
+        <v>185</v>
       </c>
       <c r="D105" s="4"/>
       <c r="E105" s="4" t="s">
-        <v>8</v>
+        <v>362</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" s="4" t="s">
-        <v>7</v>
+        <v>150</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>10</v>
+        <v>148</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>11</v>
+        <v>149</v>
       </c>
       <c r="D106" s="4"/>
       <c r="E106" s="4" t="s">
-        <v>10</v>
+        <v>348</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
@@ -3648,14 +3666,14 @@
         <v>7</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D107" s="4"/>
       <c r="E107" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
@@ -3663,14 +3681,14 @@
         <v>7</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D108" s="4"/>
       <c r="E108" s="4" t="s">
-        <v>189</v>
+        <v>10</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
@@ -3678,14 +3696,14 @@
         <v>7</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D109" s="4"/>
       <c r="E109" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
@@ -3693,14 +3711,14 @@
         <v>7</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D110" s="4"/>
       <c r="E110" s="4" t="s">
-        <v>17</v>
+        <v>189</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
@@ -3708,14 +3726,14 @@
         <v>7</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D111" s="4"/>
       <c r="E111" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
@@ -3723,14 +3741,14 @@
         <v>7</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>284</v>
+        <v>18</v>
       </c>
       <c r="D112" s="4"/>
       <c r="E112" s="4" t="s">
-        <v>95</v>
+        <v>17</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
@@ -3738,14 +3756,14 @@
         <v>7</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D113" s="4"/>
       <c r="E113" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
@@ -3753,14 +3771,14 @@
         <v>7</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>25</v>
+        <v>284</v>
       </c>
       <c r="D114" s="4"/>
       <c r="E114" s="4" t="s">
-        <v>338</v>
+        <v>95</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
@@ -3768,14 +3786,14 @@
         <v>7</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D115" s="4"/>
       <c r="E115" s="4" t="s">
-        <v>363</v>
+        <v>22</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
@@ -3783,14 +3801,14 @@
         <v>7</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D116" s="4"/>
       <c r="E116" s="4" t="s">
-        <v>364</v>
+        <v>338</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
@@ -3798,14 +3816,14 @@
         <v>7</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D117" s="4"/>
       <c r="E117" s="4" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
@@ -3813,14 +3831,14 @@
         <v>7</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D118" s="4"/>
       <c r="E118" s="4" t="s">
-        <v>32</v>
+        <v>364</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
@@ -3828,14 +3846,14 @@
         <v>7</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D119" s="4"/>
       <c r="E119" s="4" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
@@ -3843,14 +3861,14 @@
         <v>7</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D120" s="4"/>
       <c r="E120" s="4" t="s">
-        <v>367</v>
+        <v>32</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
@@ -3858,14 +3876,14 @@
         <v>7</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D121" s="4"/>
       <c r="E121" s="4" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
@@ -3873,14 +3891,14 @@
         <v>7</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D122" s="4"/>
       <c r="E122" s="4" t="s">
-        <v>40</v>
+        <v>367</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
@@ -3888,14 +3906,14 @@
         <v>7</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D123" s="4"/>
       <c r="E123" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
@@ -3903,14 +3921,14 @@
         <v>7</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C124" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D124" s="4"/>
       <c r="E124" s="4" t="s">
-        <v>370</v>
+        <v>40</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
@@ -3918,14 +3936,14 @@
         <v>7</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C125" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D125" s="4"/>
       <c r="E125" s="4" t="s">
-        <v>46</v>
+        <v>369</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
@@ -3933,44 +3951,44 @@
         <v>7</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C126" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D126" s="4"/>
       <c r="E126" s="4" t="s">
-        <v>48</v>
+        <v>370</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" s="4" t="s">
-        <v>236</v>
+        <v>7</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>237</v>
+        <v>46</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>238</v>
+        <v>47</v>
       </c>
       <c r="D127" s="4"/>
       <c r="E127" s="4" t="s">
-        <v>371</v>
+        <v>46</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" s="4" t="s">
-        <v>236</v>
+        <v>7</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>239</v>
+        <v>48</v>
       </c>
       <c r="C128" s="4" t="s">
-        <v>240</v>
+        <v>49</v>
       </c>
       <c r="D128" s="4"/>
       <c r="E128" s="4" t="s">
-        <v>372</v>
+        <v>48</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
@@ -3978,14 +3996,14 @@
         <v>236</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C129" s="4" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D129" s="4"/>
       <c r="E129" s="4" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
@@ -3993,14 +4011,14 @@
         <v>236</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>70</v>
+        <v>239</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D130" s="4"/>
       <c r="E130" s="4" t="s">
-        <v>70</v>
+        <v>372</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
@@ -4008,14 +4026,14 @@
         <v>236</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C131" s="4" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="D131" s="4"/>
       <c r="E131" s="4" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
@@ -4023,14 +4041,14 @@
         <v>236</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>246</v>
+        <v>70</v>
       </c>
       <c r="C132" s="4" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="D132" s="4"/>
       <c r="E132" s="4" t="s">
-        <v>246</v>
+        <v>70</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
@@ -4038,14 +4056,14 @@
         <v>236</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C133" s="4" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="D133" s="4"/>
       <c r="E133" s="4" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
@@ -4053,14 +4071,14 @@
         <v>236</v>
       </c>
       <c r="B134" s="4" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C134" s="4" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="D134" s="4"/>
       <c r="E134" s="4" t="s">
-        <v>375</v>
+        <v>246</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
@@ -4068,14 +4086,14 @@
         <v>236</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>21</v>
+        <v>248</v>
       </c>
       <c r="C135" s="4" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D135" s="4"/>
       <c r="E135" s="4" t="s">
-        <v>95</v>
+        <v>374</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
@@ -4083,14 +4101,14 @@
         <v>236</v>
       </c>
       <c r="B136" s="4" t="s">
-        <v>3</v>
+        <v>250</v>
       </c>
       <c r="C136" s="4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D136" s="4"/>
       <c r="E136" s="4" t="s">
-        <v>3</v>
+        <v>375</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
@@ -4098,14 +4116,14 @@
         <v>236</v>
       </c>
       <c r="B137" s="4" t="s">
-        <v>254</v>
+        <v>21</v>
       </c>
       <c r="C137" s="4" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D137" s="4"/>
       <c r="E137" s="4" t="s">
-        <v>376</v>
+        <v>95</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
@@ -4113,14 +4131,14 @@
         <v>236</v>
       </c>
       <c r="B138" s="4" t="s">
-        <v>256</v>
+        <v>3</v>
       </c>
       <c r="C138" s="4" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="D138" s="4"/>
       <c r="E138" s="4" t="s">
-        <v>256</v>
+        <v>3</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
@@ -4128,14 +4146,14 @@
         <v>236</v>
       </c>
       <c r="B139" s="4" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="C139" s="4" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="D139" s="4"/>
       <c r="E139" s="4" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
@@ -4143,14 +4161,14 @@
         <v>236</v>
       </c>
       <c r="B140" s="4" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="C140" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="D140" s="4"/>
       <c r="E140" s="4" t="s">
-        <v>379</v>
+        <v>256</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
@@ -4158,51 +4176,55 @@
         <v>236</v>
       </c>
       <c r="B141" s="4" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C141" s="4" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="D141" s="4"/>
       <c r="E141" s="4" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" s="4" t="s">
-        <v>391</v>
+        <v>236</v>
       </c>
       <c r="B142" s="4" t="s">
-        <v>392</v>
+        <v>260</v>
       </c>
       <c r="C142" s="4" t="s">
-        <v>393</v>
+        <v>261</v>
       </c>
       <c r="D142" s="4"/>
-      <c r="E142" s="4"/>
+      <c r="E142" s="4" t="s">
+        <v>379</v>
+      </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" s="4" t="s">
-        <v>391</v>
+        <v>236</v>
       </c>
       <c r="B143" s="4" t="s">
-        <v>394</v>
+        <v>262</v>
       </c>
       <c r="C143" s="4" t="s">
-        <v>395</v>
+        <v>263</v>
       </c>
       <c r="D143" s="4"/>
-      <c r="E143" s="4"/>
+      <c r="E143" s="4" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" s="4" t="s">
         <v>391</v>
       </c>
       <c r="B144" s="4" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="C144" s="4" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="D144" s="4"/>
       <c r="E144" s="4"/>
@@ -4212,10 +4234,10 @@
         <v>391</v>
       </c>
       <c r="B145" s="4" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="C145" s="4" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="D145" s="4"/>
       <c r="E145" s="4"/>
@@ -4225,10 +4247,10 @@
         <v>391</v>
       </c>
       <c r="B146" s="4" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="C146" s="4" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="D146" s="4"/>
       <c r="E146" s="4"/>
@@ -4238,10 +4260,10 @@
         <v>391</v>
       </c>
       <c r="B147" s="4" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="C147" s="4" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="D147" s="4"/>
       <c r="E147" s="4"/>
@@ -4251,10 +4273,10 @@
         <v>391</v>
       </c>
       <c r="B148" s="4" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="C148" s="4" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="D148" s="4"/>
       <c r="E148" s="4"/>
@@ -4264,10 +4286,10 @@
         <v>391</v>
       </c>
       <c r="B149" s="4" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="C149" s="4" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="D149" s="4"/>
       <c r="E149" s="4"/>
@@ -4277,10 +4299,10 @@
         <v>391</v>
       </c>
       <c r="B150" s="4" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="C150" s="4" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="D150" s="4"/>
       <c r="E150" s="4"/>
@@ -4290,10 +4312,10 @@
         <v>391</v>
       </c>
       <c r="B151" s="4" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="C151" s="4" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="D151" s="4"/>
       <c r="E151" s="4"/>
@@ -4303,10 +4325,10 @@
         <v>391</v>
       </c>
       <c r="B152" s="4" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="C152" s="4" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="D152" s="4"/>
       <c r="E152" s="4"/>
@@ -4316,36 +4338,36 @@
         <v>391</v>
       </c>
       <c r="B153" s="4" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="C153" s="4" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="D153" s="4"/>
       <c r="E153" s="4"/>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154" s="4" t="s">
-        <v>416</v>
+        <v>391</v>
       </c>
       <c r="B154" s="4" t="s">
-        <v>394</v>
+        <v>412</v>
       </c>
       <c r="C154" s="4" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="D154" s="4"/>
       <c r="E154" s="4"/>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155" s="4" t="s">
-        <v>416</v>
+        <v>391</v>
       </c>
       <c r="B155" s="4" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="C155" s="4" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="D155" s="4"/>
       <c r="E155" s="4"/>
@@ -4355,10 +4377,10 @@
         <v>416</v>
       </c>
       <c r="B156" s="4" t="s">
-        <v>420</v>
+        <v>394</v>
       </c>
       <c r="C156" s="4" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="D156" s="4"/>
       <c r="E156" s="4"/>
@@ -4368,10 +4390,10 @@
         <v>416</v>
       </c>
       <c r="B157" s="4" t="s">
-        <v>396</v>
+        <v>418</v>
       </c>
       <c r="C157" s="4" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="D157" s="4"/>
       <c r="E157" s="4"/>
@@ -4381,10 +4403,10 @@
         <v>416</v>
       </c>
       <c r="B158" s="4" t="s">
-        <v>410</v>
+        <v>420</v>
       </c>
       <c r="C158" s="4" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D158" s="4"/>
       <c r="E158" s="4"/>
@@ -4394,10 +4416,10 @@
         <v>416</v>
       </c>
       <c r="B159" s="4" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C159" s="4" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D159" s="4"/>
       <c r="E159" s="4"/>
@@ -4407,10 +4429,10 @@
         <v>416</v>
       </c>
       <c r="B160" s="4" t="s">
-        <v>425</v>
+        <v>410</v>
       </c>
       <c r="C160" s="4" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="D160" s="4"/>
       <c r="E160" s="4"/>
@@ -4420,10 +4442,10 @@
         <v>416</v>
       </c>
       <c r="B161" s="4" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="C161" s="4" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="D161" s="4"/>
       <c r="E161" s="4"/>
@@ -4433,10 +4455,10 @@
         <v>416</v>
       </c>
       <c r="B162" s="4" t="s">
-        <v>404</v>
+        <v>425</v>
       </c>
       <c r="C162" s="4" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="D162" s="4"/>
       <c r="E162" s="4"/>
@@ -4446,10 +4468,10 @@
         <v>416</v>
       </c>
       <c r="B163" s="4" t="s">
-        <v>275</v>
+        <v>406</v>
       </c>
       <c r="C163" s="4" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="D163" s="4"/>
       <c r="E163" s="4"/>
@@ -4459,10 +4481,10 @@
         <v>416</v>
       </c>
       <c r="B164" s="4" t="s">
-        <v>430</v>
+        <v>404</v>
       </c>
       <c r="C164" s="4" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="D164" s="4"/>
       <c r="E164" s="4"/>
@@ -4472,10 +4494,10 @@
         <v>416</v>
       </c>
       <c r="B165" s="4" t="s">
-        <v>402</v>
+        <v>275</v>
       </c>
       <c r="C165" s="4" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D165" s="4"/>
       <c r="E165" s="4"/>
@@ -4485,10 +4507,10 @@
         <v>416</v>
       </c>
       <c r="B166" s="4" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="C166" s="4" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="D166" s="4"/>
       <c r="E166" s="4"/>
@@ -4498,10 +4520,10 @@
         <v>416</v>
       </c>
       <c r="B167" s="4" t="s">
-        <v>271</v>
+        <v>402</v>
       </c>
       <c r="C167" s="4" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="D167" s="4"/>
       <c r="E167" s="4"/>
@@ -4511,10 +4533,10 @@
         <v>416</v>
       </c>
       <c r="B168" s="4" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="C168" s="4" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="D168" s="4"/>
       <c r="E168" s="4"/>
@@ -4524,36 +4546,36 @@
         <v>416</v>
       </c>
       <c r="B169" s="4" t="s">
-        <v>438</v>
+        <v>271</v>
       </c>
       <c r="C169" s="4" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D169" s="4"/>
       <c r="E169" s="4"/>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A170" s="4" t="s">
-        <v>440</v>
+        <v>416</v>
       </c>
       <c r="B170" s="4" t="s">
-        <v>402</v>
+        <v>436</v>
       </c>
       <c r="C170" s="4" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="D170" s="4"/>
       <c r="E170" s="4"/>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A171" s="4" t="s">
-        <v>440</v>
+        <v>416</v>
       </c>
       <c r="B171" s="4" t="s">
-        <v>408</v>
+        <v>438</v>
       </c>
       <c r="C171" s="4" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="D171" s="4"/>
       <c r="E171" s="4"/>
@@ -4563,10 +4585,10 @@
         <v>440</v>
       </c>
       <c r="B172" s="4" t="s">
-        <v>275</v>
+        <v>402</v>
       </c>
       <c r="C172" s="4" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="D172" s="4"/>
       <c r="E172" s="4"/>
@@ -4576,10 +4598,10 @@
         <v>440</v>
       </c>
       <c r="B173" s="4" t="s">
-        <v>398</v>
+        <v>408</v>
       </c>
       <c r="C173" s="4" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D173" s="4"/>
       <c r="E173" s="4"/>
@@ -4589,10 +4611,10 @@
         <v>440</v>
       </c>
       <c r="B174" s="4" t="s">
-        <v>410</v>
+        <v>275</v>
       </c>
       <c r="C174" s="4" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D174" s="4"/>
       <c r="E174" s="4"/>
@@ -4602,10 +4624,10 @@
         <v>440</v>
       </c>
       <c r="B175" s="4" t="s">
-        <v>446</v>
+        <v>398</v>
       </c>
       <c r="C175" s="4" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="D175" s="4"/>
       <c r="E175" s="4"/>
@@ -4615,10 +4637,10 @@
         <v>440</v>
       </c>
       <c r="B176" s="4" t="s">
-        <v>448</v>
+        <v>410</v>
       </c>
       <c r="C176" s="4" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="D176" s="4"/>
       <c r="E176" s="4"/>
@@ -4628,10 +4650,10 @@
         <v>440</v>
       </c>
       <c r="B177" s="4" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="C177" s="4" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="D177" s="4"/>
       <c r="E177" s="4"/>
@@ -4641,10 +4663,10 @@
         <v>440</v>
       </c>
       <c r="B178" s="4" t="s">
-        <v>406</v>
+        <v>448</v>
       </c>
       <c r="C178" s="4" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="D178" s="4"/>
       <c r="E178" s="4"/>
@@ -4654,10 +4676,10 @@
         <v>440</v>
       </c>
       <c r="B179" s="4" t="s">
-        <v>404</v>
+        <v>450</v>
       </c>
       <c r="C179" s="4" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D179" s="4"/>
       <c r="E179" s="4"/>
@@ -4667,10 +4689,10 @@
         <v>440</v>
       </c>
       <c r="B180" s="4" t="s">
-        <v>241</v>
+        <v>406</v>
       </c>
       <c r="C180" s="4" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D180" s="4"/>
       <c r="E180" s="4"/>
@@ -4680,36 +4702,36 @@
         <v>440</v>
       </c>
       <c r="B181" s="4" t="s">
-        <v>420</v>
+        <v>404</v>
       </c>
       <c r="C181" s="4" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D181" s="4"/>
       <c r="E181" s="4"/>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A182" s="4" t="s">
-        <v>273</v>
+        <v>440</v>
       </c>
       <c r="B182" s="4" t="s">
-        <v>394</v>
+        <v>241</v>
       </c>
       <c r="C182" s="4" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D182" s="4"/>
       <c r="E182" s="4"/>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A183" s="4" t="s">
-        <v>273</v>
+        <v>440</v>
       </c>
       <c r="B183" s="4" t="s">
-        <v>396</v>
+        <v>420</v>
       </c>
       <c r="C183" s="4" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="D183" s="4"/>
       <c r="E183" s="4"/>
@@ -4719,10 +4741,10 @@
         <v>273</v>
       </c>
       <c r="B184" s="4" t="s">
-        <v>420</v>
+        <v>394</v>
       </c>
       <c r="C184" s="4" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D184" s="4"/>
       <c r="E184" s="4"/>
@@ -4732,10 +4754,10 @@
         <v>273</v>
       </c>
       <c r="B185" s="4" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="C185" s="4" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="D185" s="4"/>
       <c r="E185" s="4"/>
@@ -4745,10 +4767,10 @@
         <v>273</v>
       </c>
       <c r="B186" s="4" t="s">
-        <v>460</v>
+        <v>420</v>
       </c>
       <c r="C186" s="4" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="D186" s="4"/>
       <c r="E186" s="4"/>
@@ -4758,10 +4780,10 @@
         <v>273</v>
       </c>
       <c r="B187" s="4" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C187" s="4" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="D187" s="4"/>
       <c r="E187" s="4"/>
@@ -4771,10 +4793,10 @@
         <v>273</v>
       </c>
       <c r="B188" s="4" t="s">
-        <v>274</v>
+        <v>460</v>
       </c>
       <c r="C188" s="4" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="D188" s="4"/>
       <c r="E188" s="4"/>
@@ -4784,10 +4806,10 @@
         <v>273</v>
       </c>
       <c r="B189" s="4" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C189" s="4" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D189" s="4"/>
       <c r="E189" s="4"/>
@@ -4797,10 +4819,10 @@
         <v>273</v>
       </c>
       <c r="B190" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C190" s="4" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D190" s="4"/>
       <c r="E190" s="4"/>
@@ -4810,10 +4832,10 @@
         <v>273</v>
       </c>
       <c r="B191" s="4" t="s">
-        <v>398</v>
+        <v>406</v>
       </c>
       <c r="C191" s="4" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="D191" s="4"/>
       <c r="E191" s="4"/>
@@ -4823,36 +4845,36 @@
         <v>273</v>
       </c>
       <c r="B192" s="4" t="s">
-        <v>410</v>
+        <v>275</v>
       </c>
       <c r="C192" s="4" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="D192" s="4"/>
       <c r="E192" s="4"/>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A193" s="4" t="s">
-        <v>468</v>
+        <v>273</v>
       </c>
       <c r="B193" s="4" t="s">
-        <v>469</v>
+        <v>398</v>
       </c>
       <c r="C193" s="4" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="D193" s="4"/>
       <c r="E193" s="4"/>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A194" s="4" t="s">
-        <v>468</v>
+        <v>273</v>
       </c>
       <c r="B194" s="4" t="s">
-        <v>471</v>
+        <v>410</v>
       </c>
       <c r="C194" s="4" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="D194" s="4"/>
       <c r="E194" s="4"/>
@@ -4862,10 +4884,10 @@
         <v>468</v>
       </c>
       <c r="B195" s="4" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="C195" s="4" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="D195" s="4"/>
       <c r="E195" s="4"/>
@@ -4875,10 +4897,10 @@
         <v>468</v>
       </c>
       <c r="B196" s="4" t="s">
-        <v>410</v>
+        <v>471</v>
       </c>
       <c r="C196" s="4" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="D196" s="4"/>
       <c r="E196" s="4"/>
@@ -4888,10 +4910,10 @@
         <v>468</v>
       </c>
       <c r="B197" s="4" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="C197" s="4" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="D197" s="4"/>
       <c r="E197" s="4"/>
@@ -4901,10 +4923,10 @@
         <v>468</v>
       </c>
       <c r="B198" s="4" t="s">
-        <v>275</v>
+        <v>410</v>
       </c>
       <c r="C198" s="4" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="D198" s="4"/>
       <c r="E198" s="4"/>
@@ -4914,10 +4936,10 @@
         <v>468</v>
       </c>
       <c r="B199" s="4" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="C199" s="4" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="D199" s="4"/>
       <c r="E199" s="4"/>
@@ -4927,10 +4949,10 @@
         <v>468</v>
       </c>
       <c r="B200" s="4" t="s">
-        <v>404</v>
+        <v>275</v>
       </c>
       <c r="C200" s="4" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="D200" s="4"/>
       <c r="E200" s="4"/>
@@ -4940,10 +4962,10 @@
         <v>468</v>
       </c>
       <c r="B201" s="4" t="s">
-        <v>406</v>
+        <v>479</v>
       </c>
       <c r="C201" s="4" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="D201" s="4"/>
       <c r="E201" s="4"/>
@@ -4953,10 +4975,10 @@
         <v>468</v>
       </c>
       <c r="B202" s="4" t="s">
-        <v>483</v>
+        <v>404</v>
       </c>
       <c r="C202" s="4" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="D202" s="4"/>
       <c r="E202" s="4"/>
@@ -4966,10 +4988,10 @@
         <v>468</v>
       </c>
       <c r="B203" s="4" t="s">
-        <v>398</v>
+        <v>406</v>
       </c>
       <c r="C203" s="4" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="D203" s="4"/>
       <c r="E203" s="4"/>
@@ -4979,36 +5001,36 @@
         <v>468</v>
       </c>
       <c r="B204" s="4" t="s">
-        <v>394</v>
+        <v>483</v>
       </c>
       <c r="C204" s="4" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="D204" s="4"/>
       <c r="E204" s="4"/>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A205" s="4" t="s">
-        <v>487</v>
+        <v>468</v>
       </c>
       <c r="B205" s="4" t="s">
-        <v>471</v>
+        <v>398</v>
       </c>
       <c r="C205" s="4" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="D205" s="4"/>
       <c r="E205" s="4"/>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A206" s="4" t="s">
-        <v>487</v>
+        <v>468</v>
       </c>
       <c r="B206" s="4" t="s">
-        <v>410</v>
+        <v>394</v>
       </c>
       <c r="C206" s="4" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="D206" s="4"/>
       <c r="E206" s="4"/>
@@ -5018,10 +5040,10 @@
         <v>487</v>
       </c>
       <c r="B207" s="4" t="s">
-        <v>398</v>
+        <v>471</v>
       </c>
       <c r="C207" s="4" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="D207" s="4"/>
       <c r="E207" s="4"/>
@@ -5031,10 +5053,10 @@
         <v>487</v>
       </c>
       <c r="B208" s="4" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
       <c r="C208" s="4" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="D208" s="4"/>
       <c r="E208" s="4"/>
@@ -5044,10 +5066,10 @@
         <v>487</v>
       </c>
       <c r="B209" s="4" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="C209" s="4" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="D209" s="4"/>
       <c r="E209" s="4"/>
@@ -5057,10 +5079,10 @@
         <v>487</v>
       </c>
       <c r="B210" s="4" t="s">
-        <v>493</v>
+        <v>406</v>
       </c>
       <c r="C210" s="4" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="D210" s="4"/>
       <c r="E210" s="4"/>
@@ -5070,10 +5092,10 @@
         <v>487</v>
       </c>
       <c r="B211" s="4" t="s">
-        <v>394</v>
+        <v>404</v>
       </c>
       <c r="C211" s="4" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="D211" s="4"/>
       <c r="E211" s="4"/>
@@ -5083,10 +5105,10 @@
         <v>487</v>
       </c>
       <c r="B212" s="4" t="s">
-        <v>241</v>
+        <v>493</v>
       </c>
       <c r="C212" s="4" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="D212" s="4"/>
       <c r="E212" s="4"/>
@@ -5096,36 +5118,36 @@
         <v>487</v>
       </c>
       <c r="B213" s="4" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
       <c r="C213" s="4" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="D213" s="4"/>
       <c r="E213" s="4"/>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A214" s="4" t="s">
-        <v>498</v>
+        <v>487</v>
       </c>
       <c r="B214" s="4" t="s">
-        <v>499</v>
+        <v>241</v>
       </c>
       <c r="C214" s="4" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="D214" s="4"/>
       <c r="E214" s="4"/>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A215" s="4" t="s">
-        <v>498</v>
+        <v>487</v>
       </c>
       <c r="B215" s="4" t="s">
         <v>402</v>
       </c>
       <c r="C215" s="4" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="D215" s="4"/>
       <c r="E215" s="4"/>
@@ -5135,10 +5157,10 @@
         <v>498</v>
       </c>
       <c r="B216" s="4" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="C216" s="4" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="D216" s="4"/>
       <c r="E216" s="4"/>
@@ -5148,10 +5170,10 @@
         <v>498</v>
       </c>
       <c r="B217" s="4" t="s">
-        <v>504</v>
+        <v>402</v>
       </c>
       <c r="C217" s="4" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="D217" s="4"/>
       <c r="E217" s="4"/>
@@ -5161,10 +5183,10 @@
         <v>498</v>
       </c>
       <c r="B218" s="4" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="C218" s="4" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="D218" s="4"/>
       <c r="E218" s="4"/>
@@ -5174,10 +5196,10 @@
         <v>498</v>
       </c>
       <c r="B219" s="4" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="C219" s="4" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="D219" s="4"/>
       <c r="E219" s="4"/>
@@ -5187,10 +5209,10 @@
         <v>498</v>
       </c>
       <c r="B220" s="4" t="s">
-        <v>398</v>
+        <v>506</v>
       </c>
       <c r="C220" s="4" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="D220" s="4"/>
       <c r="E220" s="4"/>
@@ -5200,10 +5222,10 @@
         <v>498</v>
       </c>
       <c r="B221" s="4" t="s">
-        <v>272</v>
+        <v>508</v>
       </c>
       <c r="C221" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="D221" s="4"/>
       <c r="E221" s="4"/>
@@ -5213,10 +5235,10 @@
         <v>498</v>
       </c>
       <c r="B222" s="4" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="C222" s="4" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="D222" s="4"/>
       <c r="E222" s="4"/>
@@ -5226,10 +5248,10 @@
         <v>498</v>
       </c>
       <c r="B223" s="4" t="s">
-        <v>450</v>
+        <v>272</v>
       </c>
       <c r="C223" s="4" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="D223" s="4"/>
       <c r="E223" s="4"/>
@@ -5239,10 +5261,10 @@
         <v>498</v>
       </c>
       <c r="B224" s="4" t="s">
-        <v>448</v>
+        <v>404</v>
       </c>
       <c r="C224" s="4" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="D224" s="4"/>
       <c r="E224" s="4"/>
@@ -5252,10 +5274,10 @@
         <v>498</v>
       </c>
       <c r="B225" s="4" t="s">
-        <v>406</v>
+        <v>450</v>
       </c>
       <c r="C225" s="4" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="D225" s="4"/>
       <c r="E225" s="4"/>
@@ -5265,10 +5287,10 @@
         <v>498</v>
       </c>
       <c r="B226" s="4" t="s">
-        <v>420</v>
+        <v>448</v>
       </c>
       <c r="C226" s="4" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="D226" s="4"/>
       <c r="E226" s="4"/>
@@ -5278,10 +5300,10 @@
         <v>498</v>
       </c>
       <c r="B227" s="4" t="s">
-        <v>241</v>
+        <v>406</v>
       </c>
       <c r="C227" s="4" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="D227" s="4"/>
       <c r="E227" s="4"/>
@@ -5291,10 +5313,10 @@
         <v>498</v>
       </c>
       <c r="B228" s="4" t="s">
-        <v>410</v>
+        <v>420</v>
       </c>
       <c r="C228" s="4" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="D228" s="4"/>
       <c r="E228" s="4"/>
@@ -5304,36 +5326,36 @@
         <v>498</v>
       </c>
       <c r="B229" s="4" t="s">
-        <v>519</v>
+        <v>241</v>
       </c>
       <c r="C229" s="4" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="D229" s="4"/>
       <c r="E229" s="4"/>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A230" s="4" t="s">
-        <v>521</v>
+        <v>498</v>
       </c>
       <c r="B230" s="4" t="s">
-        <v>522</v>
+        <v>410</v>
       </c>
       <c r="C230" s="4" t="s">
-        <v>523</v>
+        <v>518</v>
       </c>
       <c r="D230" s="4"/>
       <c r="E230" s="4"/>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A231" s="4" t="s">
-        <v>521</v>
+        <v>498</v>
       </c>
       <c r="B231" s="4" t="s">
-        <v>404</v>
+        <v>519</v>
       </c>
       <c r="C231" s="4" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="D231" s="4"/>
       <c r="E231" s="4"/>
@@ -5343,10 +5365,10 @@
         <v>521</v>
       </c>
       <c r="B232" s="4" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="C232" s="4" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="D232" s="4"/>
       <c r="E232" s="4"/>
@@ -5356,10 +5378,10 @@
         <v>521</v>
       </c>
       <c r="B233" s="4" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C233" s="4" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="D233" s="4"/>
       <c r="E233" s="4"/>
@@ -5369,83 +5391,79 @@
         <v>521</v>
       </c>
       <c r="B234" s="4" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="C234" s="4" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="D234" s="4"/>
       <c r="E234" s="4"/>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A235" s="4" t="s">
-        <v>95</v>
+        <v>521</v>
       </c>
       <c r="B235" s="4" t="s">
-        <v>265</v>
+        <v>406</v>
       </c>
       <c r="C235" s="4" t="s">
-        <v>266</v>
+        <v>527</v>
       </c>
       <c r="D235" s="4"/>
-      <c r="E235" s="4" t="s">
-        <v>352</v>
-      </c>
+      <c r="E235" s="4"/>
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A236" s="4" t="s">
-        <v>71</v>
+        <v>521</v>
       </c>
       <c r="B236" s="4" t="s">
-        <v>148</v>
+        <v>528</v>
       </c>
       <c r="C236" s="4" t="s">
-        <v>267</v>
+        <v>529</v>
       </c>
       <c r="D236" s="4"/>
-      <c r="E236" s="4" t="s">
-        <v>348</v>
-      </c>
+      <c r="E236" s="4"/>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A237" s="4" t="s">
-        <v>50</v>
+        <v>95</v>
       </c>
       <c r="B237" s="4" t="s">
-        <v>148</v>
+        <v>265</v>
       </c>
       <c r="C237" s="4" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D237" s="4"/>
       <c r="E237" s="4" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A238" s="4" t="s">
-        <v>109</v>
+        <v>71</v>
       </c>
       <c r="B238" s="4" t="s">
-        <v>265</v>
+        <v>148</v>
       </c>
       <c r="C238" s="4" t="s">
-        <v>149</v>
+        <v>267</v>
       </c>
       <c r="D238" s="4"/>
       <c r="E238" s="4" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A239" s="4" t="s">
-        <v>236</v>
+        <v>50</v>
       </c>
       <c r="B239" s="4" t="s">
         <v>148</v>
       </c>
       <c r="C239" s="4" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="D239" s="4"/>
       <c r="E239" s="4" t="s">
@@ -5454,13 +5472,13 @@
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A240" s="4" t="s">
-        <v>7</v>
+        <v>109</v>
       </c>
       <c r="B240" s="4" t="s">
         <v>265</v>
       </c>
       <c r="C240" s="4" t="s">
-        <v>269</v>
+        <v>149</v>
       </c>
       <c r="D240" s="4"/>
       <c r="E240" s="4" t="s">
@@ -5469,13 +5487,13 @@
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A241" s="4" t="s">
-        <v>7</v>
+        <v>236</v>
       </c>
       <c r="B241" s="4" t="s">
         <v>148</v>
       </c>
       <c r="C241" s="4" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D241" s="4"/>
       <c r="E241" s="4" t="s">
@@ -5484,16 +5502,46 @@
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A242" s="4" t="s">
-        <v>150</v>
+        <v>7</v>
       </c>
       <c r="B242" s="4" t="s">
-        <v>148</v>
+        <v>265</v>
       </c>
       <c r="C242" s="4" t="s">
-        <v>149</v>
+        <v>269</v>
       </c>
       <c r="D242" s="4"/>
       <c r="E242" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A243" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B243" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C243" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="D243" s="4"/>
+      <c r="E243" s="4" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A244" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B244" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C244" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="D244" s="4"/>
+      <c r="E244" s="4" t="s">
         <v>348</v>
       </c>
     </row>

</xml_diff>